<commit_message>
chore(yearly): updated desc for rowid in yearly rep
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/1_0/1_0_yearly_repeated.xlsx
+++ b/R/data/dictionaries/1_0/1_0_yearly_repeated.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/R/data/dictionaries/1_0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F02AB4-8B7D-134E-A2B5-600986331B3A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F65BF4-4F2A-8F41-B91B-C498B78D7D31}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -263,9 +263,6 @@
     <t>label</t>
   </si>
   <si>
-    <t>Unique identifier for row</t>
-  </si>
-  <si>
     <t>Age of child in years</t>
   </si>
   <si>
@@ -318,6 +315,9 @@
   </si>
   <si>
     <t>isMissing</t>
+  </si>
+  <si>
+    <t>Unique identifier for id in Opal</t>
   </si>
 </sst>
 </file>
@@ -864,8 +864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG31"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -957,7 +957,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="E2"/>
     </row>
@@ -972,7 +972,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E3"/>
     </row>
@@ -987,7 +987,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E4"/>
     </row>
@@ -1002,7 +1002,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E5"/>
     </row>
@@ -1017,7 +1017,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E6"/>
     </row>
@@ -1032,7 +1032,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E7"/>
     </row>
@@ -1047,7 +1047,7 @@
         <v>4</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E8"/>
     </row>
@@ -1077,7 +1077,7 @@
         <v>4</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E10"/>
     </row>
@@ -1107,7 +1107,7 @@
         <v>4</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E12"/>
     </row>
@@ -1137,7 +1137,7 @@
         <v>4</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E14"/>
     </row>
@@ -1167,7 +1167,7 @@
         <v>4</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E16"/>
     </row>
@@ -1197,7 +1197,7 @@
         <v>4</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E18"/>
     </row>
@@ -1227,7 +1227,7 @@
         <v>4</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E20"/>
     </row>
@@ -1242,7 +1242,7 @@
         <v>4</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E21"/>
     </row>
@@ -1257,7 +1257,7 @@
         <v>4</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E22"/>
     </row>
@@ -1272,7 +1272,7 @@
         <v>4</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E23"/>
     </row>
@@ -1287,7 +1287,7 @@
         <v>4</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E24"/>
     </row>
@@ -1302,7 +1302,7 @@
         <v>4</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E25"/>
     </row>
@@ -1409,7 +1409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A68" zoomScale="125" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A68" zoomScale="125" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C84"/>
     </sheetView>
   </sheetViews>
@@ -1429,7 +1429,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>79</v>

</xml_diff>